<commit_message>
Seguimiento a riesgos 26Julio
</commit_message>
<xml_diff>
--- a/ProjectManagement/Matriz_Riesgos.xlsx
+++ b/ProjectManagement/Matriz_Riesgos.xlsx
@@ -1,31 +1,38 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr defaultThemeVersion="164011"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="21727"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\SEI303\Documents\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Valdemar\Documents\Diplomado_SWEmbebido\_GIT_PI_DSW_UTEQ_GE\PI_DSW_UTEQ_GE\ProjectManagement\"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7574BDF1-AC7E-423B-81E4-C5102F3C3AED}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12330" activeTab="1"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Clasificación del riesgo" sheetId="2" r:id="rId1"/>
     <sheet name="Analisis de riesgos" sheetId="1" r:id="rId2"/>
   </sheets>
-  <calcPr calcId="162913"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
+    </ext>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+      </xcalcf:calcFeatures>
     </ext>
   </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="74" uniqueCount="44">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="81" uniqueCount="51">
   <si>
     <t xml:space="preserve">RIESGO </t>
   </si>
@@ -157,12 +164,44 @@
   </si>
   <si>
     <t>Se tratará de planear las actividades para que se cumplan dentro del horario</t>
+  </si>
+  <si>
+    <t>[04/Junio] No se puede utilizar la tarjeta fuera de la UTEQ, se evaluó la posibilidad de utilizar otra provista por la empresa.
+[11/Junio] Se confirmó que no será posible utilizar otra tarjeta. Se ajustará el plan para contemplar los tiempos disponibles para trabajar con la tarjeta de la UTEQ.</t>
+  </si>
+  <si>
+    <t>[07/Mayo] Se comienzan a tener juntas semanales de equipo con el asesor para analizar entregables.
+[28/Mayo] Se crea planeación considerando el tiempo restante y tomando en cuenta lo aprendido hasta el momento.
+[19/Julio] Se reevalúa la complejidad de los entregables y se solicita una prórroga para la entrega del proyecto.
+[23/Julio] Se acepta prórroga para entregar el 09 de Agosto.</t>
+  </si>
+  <si>
+    <t>[12/Julio] Pruebas demuestran error en requisito con frecuencia a utilizar.
+[19/Julio] Muestreo demuestra error con las revoluciones.
+[23/Julio] Se encuentra error y se ajusta requisito para hacer lecturas correctas.</t>
+  </si>
+  <si>
+    <t>[26/Julio] No ha sucedido el riesgo.</t>
+  </si>
+  <si>
+    <t>[12/Julio] Cambio en fecha de entrega, nueva definición de documentación y cambios menores en requisitos.
+[19/Julio] Se solicita prórroga para entrega de proyecto.
+[23/Julio] Se acepta prórroga. Se ajusta documento de requisitos y fechas de entrega considerando documentación a entregar.</t>
+  </si>
+  <si>
+    <t>[02/Julio] Se evalúa necesidad de trabajar en el proyecto días adicionales al Viernes. Cada semana se definen los días en los que el equipo podrá ir a trabajar a la UTEQ.
+[11/Julio] Trabajo en proyecto en la UTEQ
+[17/Julio] Trabajo en proyecto en la UTEQ</t>
+  </si>
+  <si>
+    <t>[28/Junio] Se hacen pruebas con potenciómetro, motor, Puente-H, Sensor. No hay daño en los componentes.
+[26/Julio] No ha sucedido el riesgo.</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="6" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -292,9 +331,6 @@
     <xf numFmtId="0" fontId="3" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="2" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -305,40 +341,45 @@
     <xf numFmtId="0" fontId="2" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="7" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="7" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" textRotation="90"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="7" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="7" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+      <alignment horizontal="left" vertical="top"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -641,153 +682,153 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="B2:H9"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="H5" sqref="H5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="3" max="3" width="16.28515625" customWidth="1"/>
-    <col min="4" max="8" width="17.7109375" customWidth="1"/>
+    <col min="3" max="3" width="16.33203125" customWidth="1"/>
+    <col min="4" max="8" width="17.6640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
-    <row r="3" spans="2:8" ht="59.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B3" s="9" t="s">
+    <row r="2" spans="2:8" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
+    <row r="3" spans="2:8" ht="59.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B3" s="18" t="s">
         <v>11</v>
       </c>
-      <c r="C3" s="10" t="s">
+      <c r="C3" s="8" t="s">
         <v>16</v>
       </c>
-      <c r="D3" s="7" t="s">
-        <v>9</v>
-      </c>
-      <c r="E3" s="7" t="s">
-        <v>9</v>
-      </c>
-      <c r="F3" s="6" t="s">
+      <c r="D3" s="6" t="s">
+        <v>9</v>
+      </c>
+      <c r="E3" s="6" t="s">
+        <v>9</v>
+      </c>
+      <c r="F3" s="5" t="s">
         <v>8</v>
       </c>
-      <c r="G3" s="6" t="s">
+      <c r="G3" s="5" t="s">
         <v>8</v>
       </c>
-      <c r="H3" s="6" t="s">
+      <c r="H3" s="5" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="4" spans="2:8" ht="59.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B4" s="9"/>
-      <c r="C4" s="10" t="s">
+    <row r="4" spans="2:8" ht="59.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B4" s="18"/>
+      <c r="C4" s="8" t="s">
         <v>15</v>
       </c>
-      <c r="D4" s="7" t="s">
-        <v>9</v>
-      </c>
-      <c r="E4" s="7" t="s">
-        <v>9</v>
-      </c>
-      <c r="F4" s="7" t="s">
-        <v>9</v>
-      </c>
-      <c r="G4" s="6" t="s">
+      <c r="D4" s="6" t="s">
+        <v>9</v>
+      </c>
+      <c r="E4" s="6" t="s">
+        <v>9</v>
+      </c>
+      <c r="F4" s="6" t="s">
+        <v>9</v>
+      </c>
+      <c r="G4" s="5" t="s">
         <v>8</v>
       </c>
-      <c r="H4" s="6" t="s">
+      <c r="H4" s="5" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="5" spans="2:8" ht="59.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B5" s="9"/>
-      <c r="C5" s="10" t="s">
+    <row r="5" spans="2:8" ht="59.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B5" s="18"/>
+      <c r="C5" s="8" t="s">
         <v>14</v>
       </c>
-      <c r="D5" s="8" t="s">
+      <c r="D5" s="7" t="s">
         <v>10</v>
       </c>
-      <c r="E5" s="7" t="s">
-        <v>9</v>
-      </c>
-      <c r="F5" s="7" t="s">
-        <v>9</v>
-      </c>
-      <c r="G5" s="7" t="s">
-        <v>9</v>
-      </c>
-      <c r="H5" s="6" t="s">
+      <c r="E5" s="6" t="s">
+        <v>9</v>
+      </c>
+      <c r="F5" s="6" t="s">
+        <v>9</v>
+      </c>
+      <c r="G5" s="6" t="s">
+        <v>9</v>
+      </c>
+      <c r="H5" s="5" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="6" spans="2:8" ht="59.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B6" s="9"/>
-      <c r="C6" s="10" t="s">
+    <row r="6" spans="2:8" ht="59.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B6" s="18"/>
+      <c r="C6" s="8" t="s">
         <v>13</v>
       </c>
-      <c r="D6" s="8" t="s">
+      <c r="D6" s="7" t="s">
         <v>10</v>
       </c>
-      <c r="E6" s="8" t="s">
+      <c r="E6" s="7" t="s">
         <v>10</v>
       </c>
-      <c r="F6" s="7" t="s">
-        <v>9</v>
-      </c>
-      <c r="G6" s="7" t="s">
-        <v>9</v>
-      </c>
-      <c r="H6" s="7" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="7" spans="2:8" ht="59.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B7" s="9"/>
-      <c r="C7" s="10" t="s">
+      <c r="F6" s="6" t="s">
+        <v>9</v>
+      </c>
+      <c r="G6" s="6" t="s">
+        <v>9</v>
+      </c>
+      <c r="H6" s="6" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="7" spans="2:8" ht="59.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B7" s="18"/>
+      <c r="C7" s="8" t="s">
         <v>12</v>
       </c>
-      <c r="D7" s="8" t="s">
+      <c r="D7" s="7" t="s">
         <v>10</v>
       </c>
-      <c r="E7" s="8" t="s">
+      <c r="E7" s="7" t="s">
         <v>10</v>
       </c>
-      <c r="F7" s="8" t="s">
+      <c r="F7" s="7" t="s">
         <v>10</v>
       </c>
-      <c r="G7" s="7" t="s">
-        <v>9</v>
-      </c>
-      <c r="H7" s="7" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="8" spans="2:8" ht="48" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="C8" s="5"/>
-      <c r="D8" s="12" t="s">
+      <c r="G7" s="6" t="s">
+        <v>9</v>
+      </c>
+      <c r="H7" s="6" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="8" spans="2:8" ht="48" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="C8" s="4"/>
+      <c r="D8" s="9" t="s">
         <v>17</v>
       </c>
-      <c r="E8" s="12" t="s">
+      <c r="E8" s="9" t="s">
         <v>18</v>
       </c>
-      <c r="F8" s="12" t="s">
+      <c r="F8" s="9" t="s">
         <v>20</v>
       </c>
-      <c r="G8" s="12" t="s">
+      <c r="G8" s="9" t="s">
         <v>19</v>
       </c>
-      <c r="H8" s="12" t="s">
+      <c r="H8" s="9" t="s">
         <v>21</v>
       </c>
     </row>
-    <row r="9" spans="2:8" ht="38.25" customHeight="1" x14ac:dyDescent="0.5">
-      <c r="D9" s="11" t="s">
+    <row r="9" spans="2:8" ht="38.25" customHeight="1" x14ac:dyDescent="0.6">
+      <c r="D9" s="19" t="s">
         <v>3</v>
       </c>
-      <c r="E9" s="11"/>
-      <c r="F9" s="11"/>
-      <c r="G9" s="11"/>
-      <c r="H9" s="11"/>
+      <c r="E9" s="19"/>
+      <c r="F9" s="19"/>
+      <c r="G9" s="19"/>
+      <c r="H9" s="19"/>
     </row>
   </sheetData>
   <mergeCells count="2">
@@ -799,40 +840,40 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:H25"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E12" sqref="E12"/>
+    <sheetView tabSelected="1" topLeftCell="B4" workbookViewId="0">
+      <selection activeCell="H8" sqref="H8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="9.5703125" customWidth="1"/>
-    <col min="2" max="2" width="33.5703125" style="15" customWidth="1"/>
-    <col min="3" max="5" width="16.28515625" style="1" customWidth="1"/>
-    <col min="6" max="6" width="32.140625" customWidth="1"/>
-    <col min="7" max="7" width="40.5703125" style="15" customWidth="1"/>
-    <col min="8" max="8" width="24.42578125" customWidth="1"/>
+    <col min="1" max="1" width="9.5546875" customWidth="1"/>
+    <col min="2" max="2" width="33.5546875" style="12" customWidth="1"/>
+    <col min="3" max="5" width="16.33203125" style="1" customWidth="1"/>
+    <col min="6" max="6" width="32.109375" customWidth="1"/>
+    <col min="7" max="7" width="40.5546875" style="12" customWidth="1"/>
+    <col min="8" max="8" width="47.44140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A1" s="4" t="s">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A1" s="20" t="s">
         <v>7</v>
       </c>
-      <c r="B1" s="4"/>
-      <c r="C1" s="4"/>
-      <c r="D1" s="4"/>
-      <c r="E1" s="4"/>
-      <c r="F1" s="4"/>
-      <c r="G1" s="4"/>
-      <c r="H1" s="4"/>
-    </row>
-    <row r="2" spans="1:8" s="2" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B1" s="20"/>
+      <c r="C1" s="20"/>
+      <c r="D1" s="20"/>
+      <c r="E1" s="20"/>
+      <c r="F1" s="20"/>
+      <c r="G1" s="20"/>
+      <c r="H1" s="20"/>
+    </row>
+    <row r="2" spans="1:8" s="2" customFormat="1" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A2" s="3" t="s">
         <v>0</v>
       </c>
-      <c r="B2" s="13" t="s">
+      <c r="B2" s="10" t="s">
         <v>1</v>
       </c>
       <c r="C2" s="3" t="s">
@@ -847,280 +888,294 @@
       <c r="F2" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="G2" s="13" t="s">
+      <c r="G2" s="10" t="s">
         <v>5</v>
       </c>
-      <c r="H2" s="13" t="s">
+      <c r="H2" s="10" t="s">
         <v>36</v>
       </c>
     </row>
-    <row r="3" spans="1:8" s="1" customFormat="1" ht="45.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A3" s="17" t="s">
+    <row r="3" spans="1:8" s="1" customFormat="1" ht="87" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A3" s="14" t="s">
         <v>22</v>
       </c>
-      <c r="B3" s="18" t="s">
+      <c r="B3" s="15" t="s">
         <v>23</v>
       </c>
-      <c r="C3" s="17">
+      <c r="C3" s="14">
         <v>5</v>
       </c>
-      <c r="D3" s="17">
+      <c r="D3" s="14">
         <v>3</v>
       </c>
-      <c r="E3" s="17">
+      <c r="E3" s="14">
         <f>C3*D3</f>
         <v>15</v>
       </c>
-      <c r="F3" s="17" t="s">
+      <c r="F3" s="14" t="s">
         <v>25</v>
       </c>
-      <c r="G3" s="19" t="s">
+      <c r="G3" s="16" t="s">
         <v>26</v>
       </c>
-      <c r="H3" s="17"/>
-    </row>
-    <row r="4" spans="1:8" ht="45.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A4" s="17" t="s">
+      <c r="H3" s="15" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="4" spans="1:8" ht="130.19999999999999" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A4" s="14" t="s">
         <v>27</v>
       </c>
-      <c r="B4" s="18" t="s">
+      <c r="B4" s="15" t="s">
         <v>28</v>
       </c>
-      <c r="C4" s="17">
+      <c r="C4" s="14">
         <v>5</v>
       </c>
-      <c r="D4" s="17">
+      <c r="D4" s="14">
         <v>3</v>
       </c>
-      <c r="E4" s="17">
-        <f t="shared" ref="E4:E32" si="0">C4*D4</f>
+      <c r="E4" s="14">
+        <f t="shared" ref="E4:E9" si="0">C4*D4</f>
         <v>15</v>
       </c>
-      <c r="F4" s="17" t="s">
+      <c r="F4" s="14" t="s">
         <v>25</v>
       </c>
-      <c r="G4" s="19" t="s">
+      <c r="G4" s="16" t="s">
         <v>40</v>
       </c>
-      <c r="H4" s="20"/>
-    </row>
-    <row r="5" spans="1:8" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A5" s="17" t="s">
+      <c r="H4" s="15" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="5" spans="1:8" ht="87" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A5" s="14" t="s">
         <v>30</v>
       </c>
-      <c r="B5" s="18" t="s">
+      <c r="B5" s="15" t="s">
         <v>29</v>
       </c>
-      <c r="C5" s="17">
+      <c r="C5" s="14">
         <v>1</v>
       </c>
-      <c r="D5" s="17">
+      <c r="D5" s="14">
         <v>2</v>
       </c>
-      <c r="E5" s="17">
+      <c r="E5" s="14">
         <f t="shared" si="0"/>
         <v>2</v>
       </c>
-      <c r="F5" s="17" t="s">
+      <c r="F5" s="14" t="s">
         <v>25</v>
       </c>
-      <c r="G5" s="19" t="s">
+      <c r="G5" s="16" t="s">
         <v>41</v>
       </c>
-      <c r="H5" s="20"/>
-    </row>
-    <row r="6" spans="1:8" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A6" s="17" t="s">
+      <c r="H5" s="15" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="6" spans="1:8" ht="29.4" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A6" s="14" t="s">
         <v>31</v>
       </c>
-      <c r="B6" s="18" t="s">
+      <c r="B6" s="15" t="s">
         <v>32</v>
       </c>
-      <c r="C6" s="17">
+      <c r="C6" s="14">
         <v>4</v>
       </c>
-      <c r="D6" s="17">
+      <c r="D6" s="14">
         <v>4</v>
       </c>
-      <c r="E6" s="17">
+      <c r="E6" s="14">
         <f t="shared" si="0"/>
         <v>16</v>
       </c>
-      <c r="F6" s="17" t="s">
+      <c r="F6" s="14" t="s">
         <v>24</v>
       </c>
-      <c r="G6" s="19" t="s">
+      <c r="G6" s="16" t="s">
         <v>42</v>
       </c>
-      <c r="H6" s="20"/>
-    </row>
-    <row r="7" spans="1:8" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A7" s="17" t="s">
+      <c r="H6" s="21" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="7" spans="1:8" ht="43.8" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A7" s="14" t="s">
         <v>37</v>
       </c>
-      <c r="B7" s="18" t="s">
+      <c r="B7" s="15" t="s">
         <v>33</v>
       </c>
-      <c r="C7" s="17">
+      <c r="C7" s="14">
         <v>2</v>
       </c>
-      <c r="D7" s="17">
+      <c r="D7" s="14">
         <v>4</v>
       </c>
-      <c r="E7" s="17">
+      <c r="E7" s="14">
         <f t="shared" si="0"/>
         <v>8</v>
       </c>
-      <c r="F7" s="17" t="s">
+      <c r="F7" s="14" t="s">
         <v>24</v>
       </c>
-      <c r="G7" s="19" t="s">
+      <c r="G7" s="16" t="s">
         <v>42</v>
       </c>
-      <c r="H7" s="20"/>
-    </row>
-    <row r="8" spans="1:8" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A8" s="17" t="s">
+      <c r="H7" s="15" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="8" spans="1:8" ht="87" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A8" s="14" t="s">
         <v>38</v>
       </c>
-      <c r="B8" s="18" t="s">
+      <c r="B8" s="15" t="s">
         <v>34</v>
       </c>
-      <c r="C8" s="17">
+      <c r="C8" s="14">
         <v>3</v>
       </c>
-      <c r="D8" s="17">
+      <c r="D8" s="14">
         <v>4</v>
       </c>
-      <c r="E8" s="17">
+      <c r="E8" s="14">
         <f t="shared" si="0"/>
         <v>12</v>
       </c>
-      <c r="F8" s="17" t="s">
+      <c r="F8" s="14" t="s">
         <v>24</v>
       </c>
-      <c r="G8" s="19" t="s">
+      <c r="G8" s="16" t="s">
         <v>42</v>
       </c>
-      <c r="H8" s="20"/>
-    </row>
-    <row r="9" spans="1:8" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A9" s="17" t="s">
+      <c r="H8" s="15" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="9" spans="1:8" ht="87" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A9" s="14" t="s">
         <v>39</v>
       </c>
-      <c r="B9" s="18" t="s">
+      <c r="B9" s="15" t="s">
         <v>35</v>
       </c>
-      <c r="C9" s="17">
+      <c r="C9" s="14">
         <v>3</v>
       </c>
-      <c r="D9" s="17">
+      <c r="D9" s="14">
         <v>3</v>
       </c>
-      <c r="E9" s="17">
+      <c r="E9" s="14">
         <f t="shared" si="0"/>
         <v>9</v>
       </c>
-      <c r="F9" s="17" t="s">
+      <c r="F9" s="14" t="s">
         <v>25</v>
       </c>
-      <c r="G9" s="19" t="s">
+      <c r="G9" s="16" t="s">
         <v>43</v>
       </c>
-      <c r="H9" s="20"/>
-    </row>
-    <row r="10" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="H9" s="15" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="10" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A10" s="1"/>
-      <c r="B10" s="14"/>
+      <c r="B10" s="11"/>
       <c r="F10" s="1"/>
-      <c r="G10" s="16"/>
-    </row>
-    <row r="11" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="G10" s="13"/>
+    </row>
+    <row r="11" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A11" s="1"/>
-      <c r="B11" s="14"/>
+      <c r="B11" s="11"/>
       <c r="F11" s="1"/>
-      <c r="G11" s="16"/>
-    </row>
-    <row r="12" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="G11" s="13"/>
+    </row>
+    <row r="12" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A12" s="1"/>
-      <c r="B12" s="14"/>
-      <c r="E12" s="21"/>
+      <c r="B12" s="11"/>
+      <c r="E12" s="17"/>
       <c r="F12" s="1"/>
-      <c r="G12" s="16"/>
-    </row>
-    <row r="13" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="G12" s="13"/>
+    </row>
+    <row r="13" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A13" s="1"/>
-      <c r="B13" s="14"/>
+      <c r="B13" s="11"/>
       <c r="F13" s="1"/>
-      <c r="G13" s="16"/>
-    </row>
-    <row r="14" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="G13" s="13"/>
+    </row>
+    <row r="14" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A14" s="1"/>
-      <c r="B14" s="14"/>
+      <c r="B14" s="11"/>
       <c r="F14" s="1"/>
-      <c r="G14" s="16"/>
-    </row>
-    <row r="15" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="G14" s="13"/>
+    </row>
+    <row r="15" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A15" s="1"/>
-      <c r="B15" s="14"/>
+      <c r="B15" s="11"/>
       <c r="F15" s="1"/>
-      <c r="G15" s="16"/>
-    </row>
-    <row r="16" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="G15" s="13"/>
+    </row>
+    <row r="16" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A16" s="1"/>
-      <c r="B16" s="14"/>
+      <c r="B16" s="11"/>
       <c r="F16" s="1"/>
-      <c r="G16" s="16"/>
-    </row>
-    <row r="17" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="G16" s="13"/>
+    </row>
+    <row r="17" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A17" s="1"/>
-      <c r="B17" s="14"/>
+      <c r="B17" s="11"/>
       <c r="F17" s="1"/>
-      <c r="G17" s="16"/>
-    </row>
-    <row r="18" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="G17" s="13"/>
+    </row>
+    <row r="18" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A18" s="1"/>
-      <c r="B18" s="14"/>
+      <c r="B18" s="11"/>
       <c r="F18" s="1"/>
-      <c r="G18" s="16"/>
-    </row>
-    <row r="19" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="G18" s="13"/>
+    </row>
+    <row r="19" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A19" s="1"/>
-      <c r="B19" s="14"/>
+      <c r="B19" s="11"/>
       <c r="F19" s="1"/>
-      <c r="G19" s="16"/>
-    </row>
-    <row r="20" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="G19" s="13"/>
+    </row>
+    <row r="20" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A20" s="1"/>
-      <c r="B20" s="14"/>
+      <c r="B20" s="11"/>
       <c r="F20" s="1"/>
-      <c r="G20" s="16"/>
-    </row>
-    <row r="21" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="G20" s="13"/>
+    </row>
+    <row r="21" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A21" s="1"/>
-      <c r="B21" s="14"/>
+      <c r="B21" s="11"/>
       <c r="F21" s="1"/>
-      <c r="G21" s="16"/>
-    </row>
-    <row r="22" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="G21" s="13"/>
+    </row>
+    <row r="22" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A22" s="1"/>
-      <c r="B22" s="14"/>
+      <c r="B22" s="11"/>
       <c r="F22" s="1"/>
-      <c r="G22" s="16"/>
-    </row>
-    <row r="23" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="G22" s="13"/>
+    </row>
+    <row r="23" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A23" s="1"/>
-      <c r="B23" s="14"/>
+      <c r="B23" s="11"/>
       <c r="F23" s="1"/>
-      <c r="G23" s="16"/>
-    </row>
-    <row r="24" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="G23" s="13"/>
+    </row>
+    <row r="24" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A24" s="1"/>
-      <c r="B24" s="14"/>
-    </row>
-    <row r="25" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="B24" s="11"/>
+    </row>
+    <row r="25" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A25" s="1"/>
-      <c r="B25" s="14"/>
+      <c r="B25" s="11"/>
     </row>
   </sheetData>
   <mergeCells count="1">

</xml_diff>